<commit_message>
fix: Se cambia para leer los numeros sin 000 a la derecha
</commit_message>
<xml_diff>
--- a/data/xlsx/resultado.xlsx
+++ b/data/xlsx/resultado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,13 +460,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>654.0549999999999</v>
+        <v>202.72</v>
       </c>
       <c r="C2" t="n">
-        <v>653.856</v>
+        <v>202.57</v>
       </c>
       <c r="D2" t="n">
-        <v>0.124</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +474,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>328.363</v>
+        <v>108.48</v>
       </c>
       <c r="C3" t="n">
-        <v>655.973</v>
+        <v>215.78</v>
       </c>
       <c r="D3" t="n">
-        <v>0.604</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>234.86</v>
+        <v>75.25</v>
       </c>
       <c r="C4" t="n">
-        <v>697.114</v>
+        <v>222.62</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9320000000000001</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>170.504</v>
+        <v>59.54</v>
       </c>
       <c r="C5" t="n">
-        <v>673.09</v>
+        <v>233.15</v>
       </c>
       <c r="D5" t="n">
-        <v>0.772</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>146.472</v>
+        <v>52.65</v>
       </c>
       <c r="C6" t="n">
-        <v>717.116</v>
+        <v>255.8</v>
       </c>
       <c r="D6" t="n">
-        <v>0.86</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>123.533</v>
+        <v>45.77</v>
       </c>
       <c r="C7" t="n">
-        <v>730.913</v>
+        <v>267.27</v>
       </c>
       <c r="D7" t="n">
-        <v>0.893</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,559 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>110.661</v>
+        <v>41.07</v>
       </c>
       <c r="C8" t="n">
-        <v>760.292</v>
+        <v>279.97</v>
       </c>
       <c r="D8" t="n">
-        <v>1.034</v>
+        <v>0.55</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>37.15</v>
+      </c>
+      <c r="C9" t="n">
+        <v>292.02</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>313.24</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>32.41</v>
+      </c>
+      <c r="C11" t="n">
+        <v>320.43</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>31.59</v>
+      </c>
+      <c r="C12" t="n">
+        <v>343.99</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>30.61</v>
+      </c>
+      <c r="C13" t="n">
+        <v>363.54</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>34.02</v>
+      </c>
+      <c r="C14" t="n">
+        <v>439.86</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>31.02</v>
+      </c>
+      <c r="C15" t="n">
+        <v>430.42</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1.14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>33.95</v>
+      </c>
+      <c r="C16" t="n">
+        <v>497.34</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>32.63</v>
+      </c>
+      <c r="C17" t="n">
+        <v>512.98</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>29.53</v>
+      </c>
+      <c r="C18" t="n">
+        <v>497.41</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>27.81</v>
+      </c>
+      <c r="C19" t="n">
+        <v>498.18</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>29.6</v>
+      </c>
+      <c r="C20" t="n">
+        <v>558.8099999999999</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>27.79</v>
+      </c>
+      <c r="C21" t="n">
+        <v>552.3200000000001</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.14</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>27.63</v>
+      </c>
+      <c r="C22" t="n">
+        <v>578.01</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>28.09</v>
+      </c>
+      <c r="C23" t="n">
+        <v>615.8099999999999</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>27.92</v>
+      </c>
+      <c r="C24" t="n">
+        <v>640.4</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>27.39</v>
+      </c>
+      <c r="C25" t="n">
+        <v>654.23</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>26.9</v>
+      </c>
+      <c r="C26" t="n">
+        <v>670.04</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.12</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>26.85</v>
+      </c>
+      <c r="C27" t="n">
+        <v>696.4</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>27.35</v>
+      </c>
+      <c r="C28" t="n">
+        <v>736.28</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>26.11</v>
+      </c>
+      <c r="C29" t="n">
+        <v>727.33</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>27.09</v>
+      </c>
+      <c r="C30" t="n">
+        <v>781.59</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>27.63</v>
+      </c>
+      <c r="C31" t="n">
+        <v>826.04</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>26.61</v>
+      </c>
+      <c r="C32" t="n">
+        <v>821.62</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>28.09</v>
+      </c>
+      <c r="C33" t="n">
+        <v>896.39</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>31.71</v>
+      </c>
+      <c r="C34" t="n">
+        <v>744.1799999999999</v>
+      </c>
+      <c r="D34" t="n">
+        <v>10.54</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>33.47</v>
+      </c>
+      <c r="C35" t="n">
+        <v>741.39</v>
+      </c>
+      <c r="D35" t="n">
+        <v>11.44</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>34.08</v>
+      </c>
+      <c r="C36" t="n">
+        <v>731.3200000000001</v>
+      </c>
+      <c r="D36" t="n">
+        <v>13.23</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>35.02</v>
+      </c>
+      <c r="C37" t="n">
+        <v>757.1900000000001</v>
+      </c>
+      <c r="D37" t="n">
+        <v>15.16</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>34.51</v>
+      </c>
+      <c r="C38" t="n">
+        <v>734.86</v>
+      </c>
+      <c r="D38" t="n">
+        <v>14.91</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>34.62</v>
+      </c>
+      <c r="C39" t="n">
+        <v>739.83</v>
+      </c>
+      <c r="D39" t="n">
+        <v>15.97</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>34.21</v>
+      </c>
+      <c r="C40" t="n">
+        <v>722.65</v>
+      </c>
+      <c r="D40" t="n">
+        <v>15.87</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>34.05</v>
+      </c>
+      <c r="C41" t="n">
+        <v>719.5700000000001</v>
+      </c>
+      <c r="D41" t="n">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="C42" t="n">
+        <v>711.88</v>
+      </c>
+      <c r="D42" t="n">
+        <v>18.94</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="n">
+        <v>34.04</v>
+      </c>
+      <c r="C43" t="n">
+        <v>718.63</v>
+      </c>
+      <c r="D43" t="n">
+        <v>18.99</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="n">
+        <v>33.74</v>
+      </c>
+      <c r="C44" t="n">
+        <v>711.64</v>
+      </c>
+      <c r="D44" t="n">
+        <v>18.82</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="n">
+        <v>33.12</v>
+      </c>
+      <c r="C45" t="n">
+        <v>701.6</v>
+      </c>
+      <c r="D45" t="n">
+        <v>20.23</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="n">
+        <v>33.85</v>
+      </c>
+      <c r="C46" t="n">
+        <v>717.16</v>
+      </c>
+      <c r="D46" t="n">
+        <v>20.86</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="n">
+        <v>33.95</v>
+      </c>
+      <c r="C47" t="n">
+        <v>716.74</v>
+      </c>
+      <c r="D47" t="n">
+        <v>20.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>